<commit_message>
fix links, title, logical models
</commit_message>
<xml_diff>
--- a/docs/omh-acceleration.xlsx
+++ b/docs/omh-acceleration.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="83">
   <si>
     <t>Path</t>
   </si>
@@ -246,11 +246,8 @@
     <t>OmhAcceleration.effectiveTimeFrame</t>
   </si>
   <si>
-    <t xml:space="preserve">dateTime|Period {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>required</t>
+    <t>dateTime {[]} {[]}
+Period {[]} {[]}</t>
   </si>
   <si>
     <t>properties.effective_time_frame</t>
@@ -261,6 +258,9 @@
   <si>
     <t xml:space="preserve">code {[]} {[]}
 </t>
+  </si>
+  <si>
+    <t>required</t>
   </si>
   <si>
     <t>http://www.fhir.org/guides/mfhir/ValueSet/body-location</t>
@@ -1324,9 +1324,11 @@
         <v>38</v>
       </c>
       <c r="W9" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X9" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="X9" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="Y9" t="s" s="2">
         <v>38</v>
       </c>
@@ -1357,7 +1359,7 @@
         <v>38</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AK9" t="s" s="2">
         <v>67</v>
@@ -1365,7 +1367,7 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -1388,7 +1390,7 @@
         <v>38</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" t="s" s="2">
@@ -1419,7 +1421,7 @@
         <v>38</v>
       </c>
       <c r="W10" t="s" s="2">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="X10" s="2"/>
       <c r="Y10" t="s" s="2">
@@ -1483,7 +1485,7 @@
         <v>38</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" t="s" s="2">
@@ -1514,7 +1516,7 @@
         <v>38</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="X11" s="2"/>
       <c r="Y11" t="s" s="2">

</xml_diff>